<commit_message>
data: complete head & face bones excel (v2)
</commit_message>
<xml_diff>
--- a/ai/data/raw/_Graduation_Project_Datas.xlsx
+++ b/ai/data/raw/_Graduation_Project_Datas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="447">
   <si>
     <t>id</t>
   </si>
@@ -70,7 +70,7 @@
 Orbitanın üst iç kısmında 2 adet sinüsü vardır.</t>
   </si>
   <si>
-    <t>Ders kitabı s.52</t>
+    <t>Ders kitabı s.54</t>
   </si>
   <si>
     <t>os_occipitale</t>
@@ -172,7 +172,7 @@
 Üzerinde alt dişlerin sıralandığı diş kemeri bulunur. </t>
   </si>
   <si>
-    <t>Ders kitabı s.53</t>
+    <t>Ders kitabı s.55</t>
   </si>
   <si>
     <t>os_vomer</t>
@@ -639,6 +639,894 @@
   </si>
   <si>
     <t>Os lacrimale, yüz kemiklerinin en küçüğü ve en incesidir.</t>
+  </si>
+  <si>
+    <t>dexter_mcq</t>
+  </si>
+  <si>
+    <t>Dexter</t>
+  </si>
+  <si>
+    <t>t_k; dexter; sağ; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi dexter terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Dexter Latince'de sağ anlamına gelir.
+B) Dexter Latince'de sol anlamına gelir.
+C) Dexter Latince'de ön anlamına gelir.
+D) Dexter Latince'de arka anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Dexter = Sağ</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.22</t>
+  </si>
+  <si>
+    <t>anterior_mcq</t>
+  </si>
+  <si>
+    <t>Anterior</t>
+  </si>
+  <si>
+    <t>t_k; anterior; ön; önde; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi anterior terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Anterior Latince'de sağ anlamına gelir.
+B) Anterior Latince'de ön/önde anlamına gelir.
+C) Anterior Latince'de sol anlamına gelir.
+D) Anterior Latince'de arka anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Anterior = Ön/Önde</t>
+  </si>
+  <si>
+    <t>superior_mcq</t>
+  </si>
+  <si>
+    <t>Superior</t>
+  </si>
+  <si>
+    <t>t_k; superior; üst; üstte; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi superior terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Superior Latince'de arka anlamına gelir.
+B) Superior Latince'de ön/önde anlamına gelir.
+C) Superior Latince'de üst/üstte anlamına gelir.
+D) Superior Latince'de sol anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Superior = Üst/Üstte</t>
+  </si>
+  <si>
+    <t>dorsalis_mcq</t>
+  </si>
+  <si>
+    <t>Dorsalis</t>
+  </si>
+  <si>
+    <t>t_k; dorsalis; sırt tarafında; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi dorsalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Dorsalis Latince'de arka anlamına gelir.
+B) Dorsalis Latince'de ön/önde anlamına gelir.
+C) Dorsalis Latince'de sırt tarafında anlamına gelir.
+D) Dorsalis Latince'de yanda anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Dorsalis = Sırt tarafında</t>
+  </si>
+  <si>
+    <t>verticalis_mcq</t>
+  </si>
+  <si>
+    <t>Verticalis</t>
+  </si>
+  <si>
+    <t>t_k; verticalis; düşey; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi verticalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Verticalis Latince'de arka anlamına gelir.
+B) Verticalis Latince'de düşey anlamına gelir.
+C) Verticalis Latince'de sırt tarafında anlamına gelir.
+D) Verticalis Latince'de yanda anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Verticalis = Düşey</t>
+  </si>
+  <si>
+    <t>medialis_mcq</t>
+  </si>
+  <si>
+    <t>Medialis</t>
+  </si>
+  <si>
+    <t>t_k; medialis; iç yan; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi medialis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Medialis Latince'de sırt tarafında anlamına gelir.
+B) Medialis Latince'de düşey anlamına gelir.
+C) Medialis Latince'de ön/önde anlamına gelir.
+D) Medialis Latince'de iç yan anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Medialis = İç yan</t>
+  </si>
+  <si>
+    <t>sagittalis_mcq</t>
+  </si>
+  <si>
+    <t>Sagittalis</t>
+  </si>
+  <si>
+    <t>t_k; sagittalis; oksal; ok yönünde; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi sagittalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Sagittalis Latince'de arka anlamına gelir.
+B) Sagittalis Latince'de düşey anlamına gelir.
+C) Sagittalis Latince'de sırt tarafında anlamına gelir.
+D) Sagittalis Latince'de oksal/ok yönünde anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Sagittalis = Oksal/Ok yönünde</t>
+  </si>
+  <si>
+    <t>proximalis_mcq</t>
+  </si>
+  <si>
+    <t>Proximalis</t>
+  </si>
+  <si>
+    <t>t_k; proximalis; gövdeye yakın; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi proximalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Proximalis Latince'de arka anlamına gelir.
+B) Proximalis Latince'de gövdeye yakın anlamına gelir.
+C) Proximalis Latince'de sırt tarafında anlamına gelir.
+D) Proximalis Latince'de oksal/ok yönünde anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Proximalis = Gövdeye yakın</t>
+  </si>
+  <si>
+    <t>centralis_mcq</t>
+  </si>
+  <si>
+    <t>Centralis</t>
+  </si>
+  <si>
+    <t>t_k; centralis; merkez; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi centralis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Centralis Latince'de merkez anlamına gelir.
+B) Centralis Latince'de gövdeye yakın anlamına gelir.
+C) Centralis Latince'de sırt tarafında anlamına gelir.
+D) Centralis Latince'de oksal/ok yönünde anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Centralis = Merkez</t>
+  </si>
+  <si>
+    <t>superficialis_mcq</t>
+  </si>
+  <si>
+    <t>Superficialis</t>
+  </si>
+  <si>
+    <t>t_k; superficialis; yüzeysel; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi superficialis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Superficialis Latince'de merkez anlamına gelir.
+B) Superficialis Latince'de yüzeysel anlamına gelir.
+C) Superficialis Latince'de sırt tarafında anlamına gelir.
+D) Superficialis Latince'de oksal/ok yönünde anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Superficialis = Yüzeysel</t>
+  </si>
+  <si>
+    <t>internalis_mcq</t>
+  </si>
+  <si>
+    <t>Internalis</t>
+  </si>
+  <si>
+    <t>t_k; internalis; iç; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi internalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Internalis Latince'de merkez anlamına gelir.
+B) Internalis Latince'de yüzeysel anlamına gelir.
+C) Internalis Latince'de sırt tarafında anlamına gelir.
+D) Internalis Latince'de iç anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Internalis = İç</t>
+  </si>
+  <si>
+    <t>cranialis_mcq</t>
+  </si>
+  <si>
+    <t>Cranialis</t>
+  </si>
+  <si>
+    <t>t_k; cranialis; baş tarafında; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi cranialis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Cranialis Latince'de merkez anlamına gelir.
+B) Cranialis Latince'de yüzeysel anlamına gelir.
+C) Cranialis Latince'de baş tarafında anlamına gelir.
+D) Cranialis Latince'de iç anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Cranialis = Baş tarafında</t>
+  </si>
+  <si>
+    <t>basalis_mcq</t>
+  </si>
+  <si>
+    <t>Basalis</t>
+  </si>
+  <si>
+    <t>t_k; basalis; taban; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi basalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Basalis Latince'de taban anlamına gelir.
+B) Basalis Latince'de yüzeysel anlamına gelir.
+C) Basalis Latince'de baş tarafında anlamına gelir.
+D) Basalis Latince'de iç anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Basalis = Taban</t>
+  </si>
+  <si>
+    <t>palmaris_mcq</t>
+  </si>
+  <si>
+    <t>Palmaris</t>
+  </si>
+  <si>
+    <t>t_k; palmaris; elin avuç içi tarafı; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi palmaris terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Palmaris Latince'de taban anlamına gelir.
+B) Palmaris Latince'de yüzeysel anlamına gelir.
+C) Palmaris Latince'de elin avuç içi anlamına gelir.
+D) Palmaris Latince'de iç anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Palmaris = Elin avuç içi tarafı</t>
+  </si>
+  <si>
+    <t>intermedius_mcq</t>
+  </si>
+  <si>
+    <t>Intermedius</t>
+  </si>
+  <si>
+    <t>t_k; intermedius; iki yapı arasında; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi intermedius terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Intermedius Latince'de iki yapı arasında anlamına gelir.
+B) Intermedius Latince'de yüzeysel anlamına gelir.
+C) Intermedius Latince'de elin avuç içi anlamına gelir.
+D) Intermedius Latince'de iç anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Intermedius = İki yapı arasında</t>
+  </si>
+  <si>
+    <t>longitudinalis_mcq</t>
+  </si>
+  <si>
+    <t>Longitudinalis</t>
+  </si>
+  <si>
+    <t>t_k; longitudinalis; uzunlamasına; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi longitudinalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Longitudinalis Latince'de uzunlamasına anlamına gelir.
+B) Longitudinalis Latince'de yüzeysel anlamına gelir.
+C) Longitudinalis Latince'de elin avuç içi anlamına gelir.
+D) Longitudinalis Latince'de iç anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Longitudinalis = Uzunlamasına</t>
+  </si>
+  <si>
+    <t>sinister_mcq</t>
+  </si>
+  <si>
+    <t>Sinister</t>
+  </si>
+  <si>
+    <t>t_k; sinister; sol; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi sinister terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Sinister Latince'de uzunlamasına anlamına gelir.
+B) Sinister Latince'de yüzeysel anlamına gelir.
+C) Sinister Latince'de elin avuç içi anlamına gelir.
+D) Sinister Latince'de sol anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Sinister = Sol</t>
+  </si>
+  <si>
+    <t>posterior_mcq</t>
+  </si>
+  <si>
+    <t>Posterior</t>
+  </si>
+  <si>
+    <t>t_k; posterior; arka; arkada; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi posterior terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Posterior Latince'de uzunlamasına anlamına gelir.
+B) Posterior Latince'de yüzeysel anlamına gelir.
+C) Posterior Latince'de arka/arkada anlamına gelir.
+D) Posterior Latince'de sol anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Posterior = Arka/Arkada</t>
+  </si>
+  <si>
+    <t>inferior_mcq</t>
+  </si>
+  <si>
+    <t>Inferior</t>
+  </si>
+  <si>
+    <t>t_k; inferior; alt; altta; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi inferior terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Inferior Latince'de uzunlamasına anlamına gelir.
+B) Inferior Latince'de alt/altta anlamına gelir.
+C) Inferior Latince'de arka/arkada anlamına gelir.
+D) Inferior Latince'de sol anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Inferior = Alt/Altta</t>
+  </si>
+  <si>
+    <t>ventralis_mcq</t>
+  </si>
+  <si>
+    <t>Ventralis</t>
+  </si>
+  <si>
+    <t>t_k; ventralis; karın tarafında; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi ventralis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Ventralis Latince'de uzunlamasına anlamına gelir.
+B) Ventralis Latince'de karın tarafında anlamına gelir.
+C) Ventralis Latince'de arka/arkada anlamına gelir.
+D) Ventralis Latince'de sol anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Ventralis = Karın tarafında</t>
+  </si>
+  <si>
+    <t>horizontalis_mcq</t>
+  </si>
+  <si>
+    <t>Horizontalis</t>
+  </si>
+  <si>
+    <t>t_k; horizontalis; yatay; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi horizontalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Horizontalis Latince'de uzunlamasına anlamına gelir.
+B) Horizontalis Latince'de karın tarafında anlamına gelir.
+C) Horizontalis Latince'de arka/arkada anlamına gelir.
+D) Horizontalis Latince'de yatay anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Horizontalis = Yatay</t>
+  </si>
+  <si>
+    <t>lateralis_mcq</t>
+  </si>
+  <si>
+    <t>Lateralis</t>
+  </si>
+  <si>
+    <t>t_k; lateralis; dış yan; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi lateralis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Lateralis Latince'de uzunlamasına anlamına gelir.
+B) Lateralis Latince'de karın tarafında anlamına gelir.
+C) Lateralis Latince'de dış yan anlamına gelir.
+D) Lateralis Latince'de yatay anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Lateralis = Dış yan</t>
+  </si>
+  <si>
+    <t>transversalis_mcq</t>
+  </si>
+  <si>
+    <t>Transversalis</t>
+  </si>
+  <si>
+    <t>t_k; transversalis; enine; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi transversalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Transversalis Latince'de uzunlamasına anlamına gelir.
+B) Transversalis Latince'de enine anlamına gelir.
+C) Transversalis Latince'de arka anlamına gelir.
+D) Transversalis Latince'de yatay anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Transversalis = Enine</t>
+  </si>
+  <si>
+    <t>distalis_mcq</t>
+  </si>
+  <si>
+    <t>Distalis</t>
+  </si>
+  <si>
+    <t>t_k; distalis; gövdeden uzak; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi distalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Distalis Latince'de gövdeden uzak anlamına gelir.
+B) Distalis Latince'de enine anlamına gelir.
+C) Distalis Latince'de arka anlamına gelir.
+D) Distalis Latince'de yatay anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Distalis = Gövdeden uzak</t>
+  </si>
+  <si>
+    <t>peripheralis_mcq</t>
+  </si>
+  <si>
+    <t>Peripheralis</t>
+  </si>
+  <si>
+    <t>t_k; peripheralis; çevre; merkezden uzak; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi peripheralis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Peripheralis Latince'de gövdeden uzak anlamına gelir.
+B) Peripheralis Latince'de enine anlamına gelir.
+C) Peripheralis Latince'de çevre/merkezden uzak anlamına gelir.
+D) Peripheralis Latince'de yatay anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Peripheralis = Çevre/Merkezden uzak</t>
+  </si>
+  <si>
+    <t>profundus_mcq</t>
+  </si>
+  <si>
+    <t>Profundus</t>
+  </si>
+  <si>
+    <t>t_k; profundus; derin; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi profundus terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Profundus Latince'de gövdeden uzak anlamına gelir.
+B) Profundus Latince'de enine anlamına gelir.
+C) Profundus Latince'de derin anlamına gelir.
+D) Profundus Latince'de yatay anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Profundus = Derin</t>
+  </si>
+  <si>
+    <t>externalis_mcq</t>
+  </si>
+  <si>
+    <t>Externalis</t>
+  </si>
+  <si>
+    <t>t_k; externalis; dış; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi externalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Externalis Latince'de gövdeden uzak anlamına gelir.
+B) Externalis Latince'de enine anlamına gelir.
+C) Externalis Latince'de çevre/merkezden uzak anlamına gelir.
+D) Externalis Latince'de dış anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Externalis = Dış</t>
+  </si>
+  <si>
+    <t>caudalis_mcq</t>
+  </si>
+  <si>
+    <t>Caudalis</t>
+  </si>
+  <si>
+    <t>t_k; caudalis; kuyruk tarafında; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi caudalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Caudalis Latince'de gövdeden uzak anlamına gelir.
+B) Caudalis Latince'de enine anlamına gelir.
+C) Caudalis Latince'de kuyruk tarafında anlamına gelir.
+D) Caudalis Latince'de dış anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Caudalis = Kuyruk tarafında</t>
+  </si>
+  <si>
+    <t>apicalis_mcq</t>
+  </si>
+  <si>
+    <t>Apicalis</t>
+  </si>
+  <si>
+    <t>t_k; apicalis; tepe; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi apicalis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Apicalis Latince'de tepe anlamına gelir.
+B) Apicalis Latince'de enine anlamına gelir.
+C) Apicalis Latince'de kuyruk tarafında anlamına gelir.
+D) Apicalis Latince'de dış anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Apicalis = Tepe</t>
+  </si>
+  <si>
+    <t>plantaris_mcq</t>
+  </si>
+  <si>
+    <t>Plantaris</t>
+  </si>
+  <si>
+    <t>t_k; plantaris; ayağın taban tarafı; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi plantaris terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Plantaris Latince'de tepe anlamına gelir.
+B) Plantaris Latince'de enine anlamına gelir.
+C) Plantaris Latince'de kuyruk tarafında anlamına gelir.
+D) Plantaris Latince'de ayağın taban tarafı anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Plantaris = Ayağın taban tarafı</t>
+  </si>
+  <si>
+    <t>contralateralis_mcq</t>
+  </si>
+  <si>
+    <t>Contralateralis</t>
+  </si>
+  <si>
+    <t>t_k; contralateralis; karşı taraf; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi contralateralis terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Contralateralis Latince'de tepe anlamına gelir.
+B) Contralateralis Latince'de karşı taraf anlamına gelir.
+C) Contralateralis Latince'de kuyruk tarafında anlamına gelir.
+D) Contralateralis Latince'de ayağın taban tarafı anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Contralateralis = Karşı taraf</t>
+  </si>
+  <si>
+    <t>obliquus_mcq</t>
+  </si>
+  <si>
+    <t>Obliquus</t>
+  </si>
+  <si>
+    <t>t_k; obliquus; eğik; çapraz; terim; anlamı; latince; yön; temel; kavram</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi obliquus terimi ile ilgili doğru bir ifadedir?</t>
+  </si>
+  <si>
+    <t>A) Obliquus Latince'de tepe anlamına gelir.
+B) Obliquus Latince'de karşı taraf anlamına gelir.
+C) Obliquus Latince'de eğik/çapraz anlamına gelir.
+D) Obliquus Latince'de ayağın taban tarafı anlamına gelir.</t>
+  </si>
+  <si>
+    <t>Obliquus = Eğik/Çapraz</t>
+  </si>
+  <si>
+    <t>mr_mcq</t>
+  </si>
+  <si>
+    <t>MR - Açılımı</t>
+  </si>
+  <si>
+    <t>t_k; mr; manyetik rezonans; görüntüleme; kısaltma</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi MR kısaltmasının açılımıdır?</t>
+  </si>
+  <si>
+    <t>A) Manyetik Rezonans Görüntüleme
+B) Mekanik Rezonans
+C) Moleküler Radyografi
+D) Manyetik Refleks Ölçümü</t>
+  </si>
+  <si>
+    <t>MR = Manyetik Rezonans Görüntüleme</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.40</t>
+  </si>
+  <si>
+    <t>bt_mcq</t>
+  </si>
+  <si>
+    <t>BT - Açılımı</t>
+  </si>
+  <si>
+    <t>t_k; bt; bilgisayarlı; tomografi; radyoloji; kısaltma</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi BT kısaltmasının açılımıdır?</t>
+  </si>
+  <si>
+    <t>A) Bilgisayarlı Tomografi
+B) Biyolojik Tarama
+C) Beyin Taraması
+D) Basınçlı Tomogram</t>
+  </si>
+  <si>
+    <t>BT = Bilgisayarlı Tomografi</t>
+  </si>
+  <si>
+    <t>ekg_mcq</t>
+  </si>
+  <si>
+    <t>EKG-Açılımı</t>
+  </si>
+  <si>
+    <t>t_k; ekg; elektrokardiyografi; kalp; elektriksel; aktivite; kısaltma</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi EKG kısaltmasının açılımıdır?</t>
+  </si>
+  <si>
+    <t>A) Elektroensefalografi
+B) Elektrokardiyografi
+C) Elektromiyografi
+D) Elektrokeratografi</t>
+  </si>
+  <si>
+    <t>EKG = Elektrokardiyografi</t>
+  </si>
+  <si>
+    <t>koah_mcq</t>
+  </si>
+  <si>
+    <t>KOAH-Açılımı</t>
+  </si>
+  <si>
+    <t>t_k; koah; kronik; obstrüktif; akciğer; hastalığı; solunum; kısaltma</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi KOAH kısaltmasının açılımıdır?</t>
+  </si>
+  <si>
+    <t>A) Kronik Obstrüktif Akciğer Hastalığı
+B) Kardiyak Oksijen Azlığı Hastalığı
+C) Kapsamlı Organik Akciğer Hasarı
+D) Kas Oksidatif Asidoz Hastalığı</t>
+  </si>
+  <si>
+    <t>KOAH = Kronik Obstrüktif Akciğer Hastalığı</t>
+  </si>
+  <si>
+    <t>dm_mcq</t>
+  </si>
+  <si>
+    <t>DM-Açılımı</t>
+  </si>
+  <si>
+    <t>t_k; dm; diabetes; mellitus; şeker; hastalığı; kısaltma</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi DM kısaltmasının açılımıdır?</t>
+  </si>
+  <si>
+    <t>A) Deri Melanomu
+B) Diz Menisküsü
+C) Diabetes Mellitus
+D) Doku Malformasyonu</t>
+  </si>
+  <si>
+    <t>DM = Diabetes Mellitus (Şeker Hastalığı)</t>
+  </si>
+  <si>
+    <t>iv_mcq</t>
+  </si>
+  <si>
+    <t>İV-Açılımı</t>
+  </si>
+  <si>
+    <t>t_k; iv; intravenöz; damar içi; uygulama; kısaltma</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi İV kısaltmasının açılımıdır?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A) İntramüsküler
+B) İntravenöz 
+C) İntraperitoneal 
+D) İntrakutanöz </t>
+  </si>
+  <si>
+    <t>İV = İntravenöz (Damar içi)</t>
+  </si>
+  <si>
+    <t>im_mcq</t>
+  </si>
+  <si>
+    <t>İM-Açılımı</t>
+  </si>
+  <si>
+    <t>t_k; im; intramüsküler; kas içi; enjeksiyon; kısaltma</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi İM kısaltmasının açılımıdır?</t>
+  </si>
+  <si>
+    <t>A) İntramüsküler 
+B) İntravasküler
+C) İntramural 
+D) İntraperitoneal</t>
+  </si>
+  <si>
+    <t>İM = İntramüsküler (Kas içi)</t>
+  </si>
+  <si>
+    <t>mi_mcq</t>
+  </si>
+  <si>
+    <t>Mİ-açılımı</t>
+  </si>
+  <si>
+    <t>t_k; mi; myokart; infarktüs; kalp krizi; kardiyak; kısaltma</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi Mİ kısaltmasının açılımıdır?</t>
+  </si>
+  <si>
+    <t>A) Myokart İnfarktüsü
+B) Mitral İnsufficiency
+C) Motor İmpuls
+D) Metabolik İnstabilite</t>
+  </si>
+  <si>
+    <t>Mİ = Myokart İnfarktüsü</t>
+  </si>
+  <si>
+    <t>ca_mcq</t>
+  </si>
+  <si>
+    <t>CA-Açılımı</t>
+  </si>
+  <si>
+    <t>t_k; ca; cancer; kanser; onkoloji; kısaltma</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi CA kısaltmasının açılımıdır?</t>
+  </si>
+  <si>
+    <t>A) Canser 
+B) Kardiyak Arrest
+C) Kalp Anomalisi
+D) Kistik Apne</t>
+  </si>
+  <si>
+    <t>CA = Canser</t>
+  </si>
+  <si>
+    <t>hb_mcq</t>
+  </si>
+  <si>
+    <t>Hb-Açılımı</t>
+  </si>
+  <si>
+    <t>t_k; hb; hemoglobin; kan; oksijen; taşıma; kısaltma</t>
+  </si>
+  <si>
+    <t>Aşağıdakilerden hangisi Hb kısaltmasının açılımıdır?</t>
+  </si>
+  <si>
+    <t>A) Hidrojen Bağlantısı
+B) Hiperbilirubin
+C) Hormon Bazı
+D) Hemoglobin</t>
+  </si>
+  <si>
+    <t>Hb = Hemoglobin</t>
   </si>
 </sst>
 </file>
@@ -1919,6 +2807,1476 @@
         <v>49</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E36" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E37" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E38" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E39" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E40" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E41" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E42" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E43" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E44" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E45" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E46" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E47" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E48" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E49" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E50" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E51" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E52" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E53" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E54" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E55" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E56" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E57" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E58" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E59" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E60" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E61" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E62" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E63" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E64" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E65" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E66" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E67" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E68" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="E69" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="E70" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="E71" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E72" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E73" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E74" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="E75" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="E76" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E77" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>